<commit_message>
Fix Gradients 2 cruise name
</commit_message>
<xml_diff>
--- a/public/example.xlsx
+++ b/public/example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisbee/Desktop/data-integration/tsdataformat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisbee/Desktop/data-integration/data-integration-uploader/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -68,9 +68,6 @@
     <t>NiskinMacroNutrients</t>
   </si>
   <si>
-    <t>MGL17-04</t>
-  </si>
-  <si>
     <t>Concentration of macronutrients collected from niskins on station.</t>
   </si>
   <si>
@@ -87,6 +84,9 @@
   </si>
   <si>
     <t>2017-05-06T20:52:57.601Z</t>
+  </si>
+  <si>
+    <t>MGL1704</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -507,12 +509,12 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -529,12 +531,12 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -568,7 +570,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -577,10 +579,10 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
         <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -602,7 +604,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>

</xml_diff>